<commit_message>
Pruebas Técnicas a los ajustes realizados
</commit_message>
<xml_diff>
--- a/FASE_2_SPRINT_3/PRUEBAS_TECNICAS/Porcentaje_Responsabilidad.xlsx
+++ b/FASE_2_SPRINT_3/PRUEBAS_TECNICAS/Porcentaje_Responsabilidad.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="807" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="807" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Caso 1" sheetId="1" r:id="rId1"/>
@@ -592,7 +592,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="43">
   <si>
     <t>Tipo Garantía Valor, Tipo Garantía Real, Tipo Garantía Fideicomiso y Tipo Garantía Aval</t>
   </si>
@@ -621,22 +621,10 @@
     <t>Real1011</t>
   </si>
   <si>
-    <t>OP200</t>
-  </si>
-  <si>
-    <t>OP300</t>
-  </si>
-  <si>
-    <t>OP400</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
     <t>Relaciones entre Garantías Fideicomiso, Garantías Reales y Garantías Valores</t>
-  </si>
-  <si>
-    <t>Fiso1012</t>
   </si>
   <si>
     <t>Escenario 3.1</t>
@@ -725,6 +713,15 @@
   <si>
     <t xml:space="preserve">AVAL-BCR201612290101 </t>
   </si>
+  <si>
+    <t>01205010001699</t>
+  </si>
+  <si>
+    <t>01205010000002</t>
+  </si>
+  <si>
+    <t>Aval-987987</t>
+  </si>
 </sst>
 </file>
 
@@ -732,9 +729,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.000000"/>
-    <numFmt numFmtId="175" formatCode="0.0000000000000000"/>
-    <numFmt numFmtId="177" formatCode="0.000000000000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000000000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1298,7 +1295,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1390,6 +1387,22 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="6" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1411,11 +1424,32 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1447,31 +1481,52 @@
     <xf numFmtId="43" fontId="0" fillId="6" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1486,52 +1541,22 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="6" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1543,73 +1568,67 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="6" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="6" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1627,27 +1646,8 @@
     <xf numFmtId="43" fontId="0" fillId="6" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="6" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1974,111 +1974,111 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="40" t="s">
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="41"/>
+      <c r="B5" s="49"/>
       <c r="C5" s="44">
         <v>55000000</v>
       </c>
       <c r="D5" s="44"/>
-      <c r="E5" s="41"/>
+      <c r="E5" s="49"/>
       <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="42">
+      <c r="G5" s="50">
         <v>19000000</v>
       </c>
-      <c r="H5" s="43"/>
+      <c r="H5" s="51"/>
       <c r="I5" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
-      <c r="B6" s="45"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="43"/>
       <c r="C6" s="44"/>
       <c r="D6" s="44"/>
-      <c r="E6" s="41"/>
+      <c r="E6" s="49"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="43"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="51"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="45"/>
-      <c r="B7" s="45"/>
+      <c r="A7" s="43"/>
+      <c r="B7" s="43"/>
       <c r="C7" s="44"/>
       <c r="D7" s="44"/>
-      <c r="E7" s="41"/>
+      <c r="E7" s="49"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="43"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="51"/>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
-      <c r="B8" s="45"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="44"/>
       <c r="D8" s="44"/>
-      <c r="E8" s="41"/>
+      <c r="E8" s="49"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="43"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="51"/>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2087,6 +2087,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="A2:I2"/>
@@ -2103,8 +2105,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2115,140 +2115,139 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="60"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="56"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="58"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="54"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="62"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="58"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="40"/>
-      <c r="H4" s="64"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="60"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="41"/>
+      <c r="A5" s="126" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="49"/>
       <c r="C5" s="44">
-        <v>55000000</v>
+        <v>35000000</v>
       </c>
       <c r="D5" s="44"/>
       <c r="E5" s="5">
         <f>(C5/$C$8)*100</f>
-        <v>60.439560439560438</v>
-      </c>
-      <c r="F5" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="47">
-        <v>19000000</v>
-      </c>
-      <c r="H5" s="48"/>
+        <v>50.359712230215827</v>
+      </c>
+      <c r="F5" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="62">
+        <v>26514845</v>
+      </c>
+      <c r="H5" s="63"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="52" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="41"/>
+      <c r="A6" s="126" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="49"/>
       <c r="C6" s="44">
-        <v>13000000</v>
+        <v>34500000</v>
       </c>
       <c r="D6" s="44"/>
       <c r="E6" s="5">
         <f t="shared" ref="E6:E7" si="0">(C6/$C$8)*100</f>
-        <v>14.285714285714285</v>
-      </c>
-      <c r="F6" s="46"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="48"/>
+        <v>49.640287769784173</v>
+      </c>
+      <c r="F6" s="61"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="63"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="41"/>
+      <c r="A7" s="67"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="44">
-        <v>23000000</v>
+        <v>0</v>
       </c>
       <c r="D7" s="44"/>
       <c r="E7" s="5">
-        <f t="shared" si="0"/>
-        <v>25.274725274725274</v>
-      </c>
-      <c r="F7" s="46"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="48"/>
+        <f>(C7/$C$8)*100</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="61"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="63"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="55">
+      <c r="A8" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="69"/>
+      <c r="C8" s="70">
         <f>SUM(C5:D7)</f>
-        <v>91000000</v>
-      </c>
-      <c r="D8" s="55"/>
+        <v>69500000</v>
+      </c>
+      <c r="D8" s="70"/>
       <c r="E8" s="6">
         <f>SUM(E5:E7)</f>
-        <v>99.999999999999986</v>
-      </c>
-      <c r="F8" s="49"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="51"/>
+        <v>100</v>
+      </c>
+      <c r="F8" s="64"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="66"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F9" s="1"/>
@@ -2256,11 +2255,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="F4:H4"/>
     <mergeCell ref="F5:F7"/>
     <mergeCell ref="G5:H7"/>
     <mergeCell ref="F8:H8"/>
@@ -2272,6 +2266,11 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2296,92 +2295,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="60"/>
+      <c r="A1" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="56"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="58"/>
+      <c r="A2" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="54"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="62"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="58"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="63" t="s">
+      <c r="A4" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="40" t="s">
+      <c r="F4" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="64"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="60"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="75">
+      <c r="A5" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="75"/>
+      <c r="C5" s="80">
         <v>3000000</v>
       </c>
-      <c r="D5" s="76"/>
+      <c r="D5" s="81"/>
       <c r="E5" s="13">
         <f>(K5/$K$9)*100</f>
         <v>57.786272641973454</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G5" s="11">
         <v>100</v>
       </c>
-      <c r="H5" s="47">
+      <c r="H5" s="62">
         <v>46802442.600000001</v>
       </c>
-      <c r="I5" s="47"/>
+      <c r="I5" s="62"/>
       <c r="J5" s="9">
         <f>(H5*G5)/100</f>
         <v>46802442.600000001</v>
@@ -2392,24 +2391,24 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="71"/>
-      <c r="B6" s="72"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="78"/>
+      <c r="A6" s="76"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="83"/>
       <c r="E6" s="13">
         <f t="shared" ref="E6:E7" si="0">(K6/$K$9)*100</f>
         <v>14.374741979546785</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G6" s="11">
         <v>43.89</v>
       </c>
-      <c r="H6" s="67">
+      <c r="H6" s="89">
         <v>26526400</v>
       </c>
-      <c r="I6" s="68"/>
+      <c r="I6" s="90"/>
       <c r="J6" s="9">
         <f>(H6*G6)/100</f>
         <v>11642436.960000001</v>
@@ -2420,24 +2419,24 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="71"/>
-      <c r="B7" s="72"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="78"/>
+      <c r="A7" s="76"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="83"/>
       <c r="E7" s="13">
         <f t="shared" si="0"/>
         <v>27.838985378479759</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G7" s="11">
         <v>85</v>
       </c>
-      <c r="H7" s="47">
+      <c r="H7" s="62">
         <v>26526400</v>
       </c>
-      <c r="I7" s="47"/>
+      <c r="I7" s="62"/>
       <c r="J7" s="9">
         <f t="shared" ref="J7:J8" si="1">(H7*G7)/100</f>
         <v>22547440</v>
@@ -2448,24 +2447,24 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="73"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="80"/>
+      <c r="A8" s="78"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="85"/>
       <c r="E8" s="13">
         <f t="shared" ref="E8" si="3">(K8/$K$9)*100</f>
         <v>0</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G8" s="11">
         <v>0</v>
       </c>
-      <c r="H8" s="47">
+      <c r="H8" s="62">
         <v>250000</v>
       </c>
-      <c r="I8" s="47"/>
+      <c r="I8" s="62"/>
       <c r="J8" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2476,23 +2475,23 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="55">
+      <c r="A9" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="69"/>
+      <c r="C9" s="70">
         <f>SUM(C5:D7)</f>
         <v>3000000</v>
       </c>
-      <c r="D9" s="55"/>
+      <c r="D9" s="70"/>
       <c r="E9" s="6">
         <f>SUM(E5:E8)</f>
         <v>100</v>
       </c>
-      <c r="F9" s="65"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="66"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
       <c r="J9" s="14">
         <f>SUM(J5:J8)</f>
         <v>80992319.560000002</v>
@@ -2511,11 +2510,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="F4:K4"/>
-    <mergeCell ref="H5:I5"/>
     <mergeCell ref="H8:I8"/>
     <mergeCell ref="A5:B8"/>
     <mergeCell ref="C5:D8"/>
@@ -2525,6 +2519,11 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H7:I7"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="F4:K4"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2551,64 +2550,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="60"/>
+      <c r="A1" s="55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="56"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="58"/>
+      <c r="A2" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="54"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="62"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="58"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="92"/>
-      <c r="C4" s="84" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="92"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="73" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="95"/>
       <c r="E4" s="28" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>4</v>
@@ -2617,29 +2616,29 @@
         <v>6</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="84" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="92"/>
+        <v>15</v>
+      </c>
+      <c r="I4" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="95"/>
       <c r="K4" s="27" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="69" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="75">
+      <c r="A5" s="74" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="75"/>
+      <c r="C5" s="80">
         <v>3000000</v>
       </c>
-      <c r="D5" s="76"/>
-      <c r="E5" s="85">
+      <c r="D5" s="81"/>
+      <c r="E5" s="97">
         <f>C5-L5</f>
         <v>1683300</v>
       </c>
@@ -2648,38 +2647,38 @@
         <v>43.89</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H5" s="11">
         <v>43.89</v>
       </c>
-      <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
       <c r="L5" s="9">
         <f>(C5*H5)/100</f>
         <v>1316700</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="71"/>
-      <c r="B6" s="72"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="86"/>
+      <c r="A6" s="76"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="98"/>
       <c r="F6" s="5">
         <f>(L6/$L$9)*100</f>
         <v>37.765083414082952</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H6" s="11">
         <v>100</v>
       </c>
-      <c r="I6" s="47">
+      <c r="I6" s="62">
         <v>46802442.600000001</v>
       </c>
-      <c r="J6" s="47"/>
+      <c r="J6" s="62"/>
       <c r="K6" s="9">
         <f>(I6*H6)/100</f>
         <v>46802442.600000001</v>
@@ -2690,25 +2689,25 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="71"/>
-      <c r="B7" s="72"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="86"/>
+      <c r="A7" s="76"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="98"/>
       <c r="F7" s="5">
         <f>(L7/$L$9)*100</f>
         <v>18.193622064802888</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H7" s="11">
         <v>85</v>
       </c>
-      <c r="I7" s="47">
+      <c r="I7" s="62">
         <v>26526400</v>
       </c>
-      <c r="J7" s="47"/>
+      <c r="J7" s="62"/>
       <c r="K7" s="9">
         <f>(I7*H7)/100</f>
         <v>22547440</v>
@@ -2719,25 +2718,25 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="73"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="80"/>
-      <c r="E8" s="87"/>
+      <c r="A8" s="78"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="99"/>
       <c r="F8" s="5">
         <f>(L8/$L$9)*100</f>
         <v>0.15129452111417263</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H8" s="11">
         <v>75</v>
       </c>
-      <c r="I8" s="47">
+      <c r="I8" s="62">
         <v>250000</v>
       </c>
-      <c r="J8" s="47"/>
+      <c r="J8" s="62"/>
       <c r="K8" s="9">
         <f>(I8*H8)/100</f>
         <v>187500</v>
@@ -2748,24 +2747,24 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="88" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="89"/>
-      <c r="C9" s="90">
+      <c r="A9" s="91" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="92"/>
+      <c r="C9" s="93">
         <f>SUM(C5:D7)</f>
         <v>3000000</v>
       </c>
-      <c r="D9" s="91"/>
+      <c r="D9" s="94"/>
       <c r="E9" s="25"/>
       <c r="F9" s="19">
         <f>SUM(F5:F8)</f>
         <v>100.00000000000001</v>
       </c>
-      <c r="G9" s="65"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="66"/>
-      <c r="J9" s="66"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="88"/>
       <c r="K9" s="17">
         <f>SUM(K5:K8)</f>
         <v>69537382.599999994</v>
@@ -2784,6 +2783,9 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:L3"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="G9:J9"/>
@@ -2797,9 +2799,6 @@
     <mergeCell ref="A5:B8"/>
     <mergeCell ref="C5:D8"/>
     <mergeCell ref="E5:E8"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2832,65 +2831,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="60"/>
+      <c r="A1" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="56"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="58"/>
+      <c r="A2" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="54"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="62"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="58"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="106" t="s">
+      <c r="A4" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="107"/>
-      <c r="C4" s="108" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="107"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="107" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="106"/>
       <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
@@ -2898,48 +2897,48 @@
         <v>6</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="84" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="95"/>
+      <c r="J4" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="92"/>
-      <c r="J4" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>24</v>
-      </c>
       <c r="L4" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="116" t="s">
-        <v>36</v>
+      <c r="A5" s="108" t="s">
+        <v>32</v>
       </c>
       <c r="B5" s="109"/>
-      <c r="C5" s="75">
+      <c r="C5" s="80">
         <v>27069500</v>
       </c>
-      <c r="D5" s="76"/>
+      <c r="D5" s="81"/>
       <c r="E5" s="5">
         <f>(M5/$M$9)*100</f>
         <v>74.457136332671368</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G5" s="11">
         <v>100</v>
       </c>
-      <c r="H5" s="47">
+      <c r="H5" s="62">
         <v>21942042.829999998</v>
       </c>
-      <c r="I5" s="47"/>
+      <c r="I5" s="62"/>
       <c r="J5" s="9">
         <f>(H5*C18)/100</f>
         <v>21942042.829999998</v>
@@ -2951,30 +2950,30 @@
         <f>J5-F24</f>
         <v>-2549660457.1700001</v>
       </c>
-      <c r="M5" s="123">
+      <c r="M5" s="42">
         <f>(L5/$L$9)*$C$5</f>
         <v>20155174.519572478</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="117"/>
-      <c r="B6" s="110"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="78"/>
+      <c r="A6" s="110"/>
+      <c r="B6" s="111"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="83"/>
       <c r="E6" s="5">
         <f t="shared" ref="E6:E7" si="0">(M6/$M$9)*100</f>
         <v>23.370696822445808</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G6" s="11">
         <v>85</v>
       </c>
-      <c r="H6" s="47">
+      <c r="H6" s="62">
         <v>14960000</v>
       </c>
-      <c r="I6" s="47"/>
+      <c r="I6" s="62"/>
       <c r="J6" s="9">
         <f>(H6*C19)/100</f>
         <v>11794464</v>
@@ -2986,31 +2985,31 @@
         <f>J6-F25</f>
         <v>-800290536</v>
       </c>
-      <c r="M6" s="123">
+      <c r="M6" s="42">
         <f>(L6/$L$9)*$C$5</f>
         <v>6326330.7763519678</v>
       </c>
-      <c r="N6" s="121"/>
+      <c r="N6" s="40"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="117"/>
-      <c r="B7" s="110"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="78"/>
+      <c r="A7" s="110"/>
+      <c r="B7" s="111"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="83"/>
       <c r="E7" s="5">
         <f t="shared" si="0"/>
         <v>-0.16850246222104373</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G7" s="11">
         <v>75.650000000000006</v>
       </c>
-      <c r="H7" s="47">
+      <c r="H7" s="62">
         <v>28695164.199999999</v>
       </c>
-      <c r="I7" s="47"/>
+      <c r="I7" s="62"/>
       <c r="J7" s="9">
         <f>(H7*C20)/100</f>
         <v>21707891.717300002</v>
@@ -3022,30 +3021,30 @@
         <f>J7-F26</f>
         <v>5770085.7973000016</v>
       </c>
-      <c r="M7" s="123">
+      <c r="M7" s="42">
         <f>(L7/$L$9)*$C$5</f>
         <v>-45612.77401092543</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="117"/>
-      <c r="B8" s="110"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="78"/>
+      <c r="A8" s="110"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="5">
         <f t="shared" ref="E8" si="1">(M8/$M$9)*100</f>
         <v>2.3406693071038576</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G8" s="11">
         <v>75</v>
       </c>
-      <c r="H8" s="47">
+      <c r="H8" s="62">
         <v>145778911</v>
       </c>
-      <c r="I8" s="47"/>
+      <c r="I8" s="62"/>
       <c r="J8" s="9">
         <f>(H8*C21)/100</f>
         <v>109334183.25</v>
@@ -3057,12 +3056,12 @@
         <f>J8-F27</f>
         <v>-80152316.75</v>
       </c>
-      <c r="M8" s="123">
+      <c r="M8" s="42">
         <f>(L8/$L$9)*$C$5</f>
         <v>633607.47808647878</v>
       </c>
-      <c r="N8" s="119"/>
-      <c r="O8" s="118"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="37"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="102"/>
@@ -3076,10 +3075,10 @@
         <f>SUM(E5:E8)</f>
         <v>99.999999999999986</v>
       </c>
-      <c r="F9" s="65"/>
-      <c r="G9" s="66"/>
-      <c r="H9" s="66"/>
-      <c r="I9" s="66"/>
+      <c r="F9" s="87"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
       <c r="J9" s="17">
         <f>SUM(J5:J8)</f>
         <v>164778581.79729998</v>
@@ -3089,20 +3088,20 @@
         <f>SUM(L5:L8)</f>
         <v>-3424333224.1227002</v>
       </c>
-      <c r="M9" s="122">
+      <c r="M9" s="41">
         <f>SUM(M5:M8)</f>
         <v>27069500</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="106" t="s">
+      <c r="A10" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="107"/>
-      <c r="C10" s="108" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="107"/>
+      <c r="B10" s="106"/>
+      <c r="C10" s="107" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="106"/>
       <c r="E10" s="4" t="s">
         <v>4</v>
       </c>
@@ -3110,48 +3109,48 @@
         <v>6</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10" s="84" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="95"/>
+      <c r="J10" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="I10" s="92"/>
-      <c r="J10" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="16" t="s">
-        <v>24</v>
-      </c>
       <c r="L10" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="105" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="105"/>
-      <c r="C11" s="47">
+      <c r="A11" s="112" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="112"/>
+      <c r="C11" s="62">
         <v>11152634</v>
       </c>
-      <c r="D11" s="47"/>
+      <c r="D11" s="62"/>
       <c r="E11" s="5">
         <f>(M11/$M$15)*100</f>
         <v>95.18991817231624</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G11" s="11">
         <v>100</v>
       </c>
-      <c r="H11" s="47">
+      <c r="H11" s="62">
         <v>21942042.829999998</v>
       </c>
-      <c r="I11" s="47"/>
+      <c r="I11" s="62"/>
       <c r="J11" s="9">
         <f>(H11*C18)/100</f>
         <v>21942042.829999998</v>
@@ -3169,24 +3168,24 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="105"/>
-      <c r="B12" s="105"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="47"/>
+      <c r="A12" s="112"/>
+      <c r="B12" s="112"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
       <c r="E12" s="5">
         <f>(M12/$M$15)*100</f>
         <v>-0.16242131270311336</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G12" s="11">
         <v>78.84</v>
       </c>
-      <c r="H12" s="47">
+      <c r="H12" s="62">
         <v>14960000</v>
       </c>
-      <c r="I12" s="47"/>
+      <c r="I12" s="62"/>
       <c r="J12" s="9">
         <f>(H12*C19)/100</f>
         <v>11794464</v>
@@ -3204,24 +3203,24 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="105"/>
-      <c r="B13" s="105"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
+      <c r="A13" s="112"/>
+      <c r="B13" s="112"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
       <c r="E13" s="5">
         <f>(M13/$M$15)*100</f>
         <v>-0.32224517081351589</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G13" s="11">
         <v>85</v>
       </c>
-      <c r="H13" s="47">
+      <c r="H13" s="62">
         <v>28695164.199999999</v>
       </c>
-      <c r="I13" s="47"/>
+      <c r="I13" s="62"/>
       <c r="J13" s="9">
         <f>(H13*C20)/100</f>
         <v>21707891.717300002</v>
@@ -3239,24 +3238,24 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="105"/>
-      <c r="B14" s="105"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
+      <c r="A14" s="112"/>
+      <c r="B14" s="112"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
       <c r="E14" s="5">
         <f>(M14/$M$15)*100</f>
         <v>5.294748311200399</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G14" s="11">
         <v>80</v>
       </c>
-      <c r="H14" s="47">
+      <c r="H14" s="62">
         <v>145778911</v>
       </c>
-      <c r="I14" s="47"/>
+      <c r="I14" s="62"/>
       <c r="J14" s="9">
         <f>(H14*C21)/100</f>
         <v>109334183.25</v>
@@ -3285,10 +3284,10 @@
         <f>SUM(E11:E14)</f>
         <v>100</v>
       </c>
-      <c r="F15" s="49"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="50"/>
-      <c r="I15" s="50"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="65"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
       <c r="J15" s="21">
         <f>SUM(J11:J14)</f>
         <v>164778581.79729998</v>
@@ -3304,75 +3303,75 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="97" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="98"/>
-      <c r="C17" s="99"/>
+      <c r="A17" s="113" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="114"/>
+      <c r="C17" s="115"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="96" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="96"/>
+      <c r="A18" s="100" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="100"/>
       <c r="C18" s="32">
         <f>MIN(G5,G11)</f>
         <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="100" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="101"/>
+      <c r="A19" s="116" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="117"/>
       <c r="C19" s="32">
         <v>78.84</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="96" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="96"/>
+      <c r="A20" s="100" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="100"/>
       <c r="C20" s="32">
         <f>MIN(G7)</f>
         <v>75.650000000000006</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="96" t="s">
-        <v>41</v>
-      </c>
-      <c r="B21" s="96"/>
+      <c r="A21" s="100" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="100"/>
       <c r="C21" s="32">
         <f>MIN(G8)</f>
         <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="95" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="95"/>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
+      <c r="A23" s="118" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="118"/>
+      <c r="C23" s="118"/>
+      <c r="D23" s="118"/>
       <c r="E23" s="33" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F23" s="33" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="94">
+        <v>34</v>
+      </c>
+      <c r="B24" s="101">
         <f>SUM(K5,K11)</f>
         <v>5007857500</v>
       </c>
-      <c r="C24" s="94"/>
-      <c r="D24" s="94"/>
+      <c r="C24" s="101"/>
+      <c r="D24" s="101"/>
       <c r="E24" s="34">
         <f>K5</f>
         <v>2436255000</v>
@@ -3384,14 +3383,14 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="94">
+        <v>35</v>
+      </c>
+      <c r="B25" s="101">
         <f>SUM(K6,K12)</f>
         <v>819759953.37</v>
       </c>
-      <c r="C25" s="94"/>
-      <c r="D25" s="94"/>
+      <c r="C25" s="101"/>
+      <c r="D25" s="101"/>
       <c r="E25" s="34">
         <f>K6</f>
         <v>7674953.3700000001</v>
@@ -3403,14 +3402,14 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="94">
+        <v>36</v>
+      </c>
+      <c r="B26" s="101">
         <f>SUM(K7,K13)</f>
         <v>29472555.920000002</v>
       </c>
-      <c r="C26" s="94"/>
-      <c r="D26" s="94"/>
+      <c r="C26" s="101"/>
+      <c r="D26" s="101"/>
       <c r="E26" s="34">
         <f>K7</f>
         <v>13534750</v>
@@ -3422,14 +3421,14 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="94">
+        <v>37</v>
+      </c>
+      <c r="B27" s="101">
         <f>SUM(K8,K14)</f>
         <v>433112000</v>
       </c>
-      <c r="C27" s="94"/>
-      <c r="D27" s="94"/>
+      <c r="C27" s="101"/>
+      <c r="D27" s="101"/>
       <c r="E27" s="34">
         <f>K8</f>
         <v>243625500</v>
@@ -3441,33 +3440,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="C5:D8"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="A2:M2"/>
-    <mergeCell ref="A1:M1"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="A5:B8"/>
-    <mergeCell ref="C11:D14"/>
-    <mergeCell ref="A11:B14"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="A17:C17"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C15:D15"/>
@@ -3478,6 +3450,33 @@
     <mergeCell ref="A23:D23"/>
     <mergeCell ref="A18:B18"/>
     <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="C5:D8"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="F9:I9"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="A5:B8"/>
+    <mergeCell ref="C11:D14"/>
+    <mergeCell ref="A11:B14"/>
+    <mergeCell ref="H10:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3489,7 +3488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
@@ -3510,70 +3509,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="59" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="60"/>
+      <c r="A1" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="56"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="58"/>
+      <c r="A2" s="52" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="54"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="61" t="s">
+      <c r="A3" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="62"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="58"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="106" t="s">
+      <c r="A4" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="107"/>
-      <c r="C4" s="108" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="107"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="107" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="106"/>
       <c r="E4" s="28" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>4</v>
@@ -3582,35 +3581,35 @@
         <v>6</v>
       </c>
       <c r="H4" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="84" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="95"/>
+      <c r="K4" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="92"/>
-      <c r="K4" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="L4" s="16" t="s">
-        <v>24</v>
-      </c>
       <c r="M4" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="111" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="70"/>
-      <c r="C5" s="75">
+      <c r="A5" s="121" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="75"/>
+      <c r="C5" s="80">
         <v>27069500</v>
       </c>
-      <c r="D5" s="76"/>
-      <c r="E5" s="85">
+      <c r="D5" s="81"/>
+      <c r="E5" s="97">
         <f>C5-I9</f>
         <v>9474325</v>
       </c>
@@ -3619,15 +3618,15 @@
         <v>25.940828789986288</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H5" s="11">
         <v>100</v>
       </c>
-      <c r="I5" s="47">
+      <c r="I5" s="62">
         <v>21942042.829999998</v>
       </c>
-      <c r="J5" s="47"/>
+      <c r="J5" s="62"/>
       <c r="K5" s="9">
         <f>(I5*H5)/100</f>
         <v>21942042.829999998</v>
@@ -3645,25 +3644,25 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="112"/>
-      <c r="B6" s="72"/>
-      <c r="C6" s="77"/>
-      <c r="D6" s="78"/>
-      <c r="E6" s="86"/>
+      <c r="A6" s="122"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="98"/>
       <c r="F6" s="5">
         <f t="shared" ref="F6:F8" si="0">(N6/$N$10)*100</f>
         <v>8.302389375501166</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H6" s="11">
         <v>85</v>
       </c>
-      <c r="I6" s="47">
+      <c r="I6" s="62">
         <v>14960000</v>
       </c>
-      <c r="J6" s="47"/>
+      <c r="J6" s="62"/>
       <c r="K6" s="9">
         <f>(I6*C25)/100</f>
         <v>9327560</v>
@@ -3681,25 +3680,25 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="112"/>
-      <c r="B7" s="72"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="86"/>
+      <c r="A7" s="122"/>
+      <c r="B7" s="77"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="98"/>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
         <v>-5.8706172953487831E-2</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H7" s="11">
         <v>75.650000000000006</v>
       </c>
-      <c r="I7" s="47">
+      <c r="I7" s="62">
         <v>28695164.199999999</v>
       </c>
-      <c r="J7" s="47"/>
+      <c r="J7" s="62"/>
       <c r="K7" s="9">
         <f>(I7*C26)/100</f>
         <v>21707891.717300002</v>
@@ -3712,30 +3711,30 @@
         <v>5770085.7973000016</v>
       </c>
       <c r="N7" s="10">
-        <f t="shared" ref="N7:N9" si="2">(M7/$M$10)*$E$5</f>
+        <f t="shared" ref="N7:N8" si="2">(M7/$M$10)*$E$5</f>
         <v>-15891.467487644388</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="112"/>
-      <c r="B8" s="72"/>
-      <c r="C8" s="77"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="86"/>
+      <c r="A8" s="122"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="83"/>
+      <c r="E8" s="98"/>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
         <v>0.81548800746603389</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H8" s="11">
         <v>75</v>
       </c>
-      <c r="I8" s="47">
+      <c r="I8" s="62">
         <v>145778911</v>
       </c>
-      <c r="J8" s="47"/>
+      <c r="J8" s="62"/>
       <c r="K8" s="9">
         <f>(I8*C27)/100</f>
         <v>109334183.25</v>
@@ -3751,29 +3750,29 @@
         <f t="shared" si="2"/>
         <v>220748.52618101804</v>
       </c>
-      <c r="O8" s="120"/>
+      <c r="O8" s="39"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="112"/>
-      <c r="B9" s="72"/>
-      <c r="C9" s="77"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="86"/>
+      <c r="A9" s="122"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="98"/>
       <c r="F9" s="5">
         <f>H9</f>
         <v>65</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H9" s="11">
         <v>65</v>
       </c>
-      <c r="I9" s="47">
+      <c r="I9" s="62">
         <f>(H9*C5)/100</f>
         <v>17595175</v>
       </c>
-      <c r="J9" s="47"/>
+      <c r="J9" s="62"/>
       <c r="K9" s="9"/>
       <c r="L9" s="12">
         <v>8120850</v>
@@ -3788,8 +3787,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="50"/>
-      <c r="B10" s="113"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="123"/>
       <c r="C10" s="104">
         <f>SUM(C5:D7)</f>
         <v>27069500</v>
@@ -3800,10 +3799,10 @@
         <f>SUM(F5:F9)</f>
         <v>100</v>
       </c>
-      <c r="G10" s="65"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="66"/>
+      <c r="G10" s="87"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="88"/>
       <c r="K10" s="17">
         <f>SUM(K5:K7)</f>
         <v>52977494.547299996</v>
@@ -3819,14 +3818,14 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="106" t="s">
+      <c r="A11" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="107"/>
-      <c r="C11" s="108" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="107"/>
+      <c r="B11" s="106"/>
+      <c r="C11" s="107" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="106"/>
       <c r="E11" s="30"/>
       <c r="F11" s="4" t="s">
         <v>4</v>
@@ -3835,35 +3834,35 @@
         <v>6</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="84" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="95"/>
+      <c r="K11" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="J11" s="92"/>
-      <c r="K11" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="L11" s="16" t="s">
-        <v>24</v>
-      </c>
       <c r="M11" s="16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="111" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" s="70"/>
-      <c r="C12" s="75">
+      <c r="A12" s="121" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="75"/>
+      <c r="C12" s="80">
         <v>11152634</v>
       </c>
-      <c r="D12" s="76"/>
-      <c r="E12" s="85">
+      <c r="D12" s="81"/>
+      <c r="E12" s="97">
         <f>C12-I16</f>
         <v>3904537.1634</v>
       </c>
@@ -3872,15 +3871,15 @@
         <v>33.120566746795248</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H12" s="11">
         <v>100</v>
       </c>
-      <c r="I12" s="47">
+      <c r="I12" s="62">
         <v>21942042.829999998</v>
       </c>
-      <c r="J12" s="47"/>
+      <c r="J12" s="62"/>
       <c r="K12" s="9">
         <f>(I12*C24)/100</f>
         <v>21942042.829999998</v>
@@ -3898,25 +3897,25 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="112"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="77"/>
-      <c r="D13" s="78"/>
-      <c r="E13" s="86"/>
+      <c r="A13" s="122"/>
+      <c r="B13" s="77"/>
+      <c r="C13" s="82"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="98"/>
       <c r="F13" s="5">
         <f t="shared" ref="F13:F15" si="3">(N13/$N$17)*100</f>
         <v>0.15929076204617018</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H13" s="11">
         <v>78.84</v>
       </c>
-      <c r="I13" s="47">
+      <c r="I13" s="62">
         <v>14960000</v>
       </c>
-      <c r="J13" s="47"/>
+      <c r="J13" s="62"/>
       <c r="K13" s="9">
         <f t="shared" ref="K13:K15" si="4">(I13*C25)/100</f>
         <v>9327560</v>
@@ -3929,30 +3928,30 @@
         <v>-11611448.370000001</v>
       </c>
       <c r="N13" s="10">
-        <f t="shared" ref="N13:N16" si="6">(M13/$M$17)*$E$12</f>
+        <f t="shared" ref="N13:N15" si="6">(M13/$M$17)*$E$12</f>
         <v>17765.115686820271</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="112"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="77"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="86"/>
+      <c r="A14" s="122"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="98"/>
       <c r="F14" s="5">
         <f t="shared" si="3"/>
         <v>-0.11212261648802914</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H14" s="11">
         <v>85</v>
       </c>
-      <c r="I14" s="47">
+      <c r="I14" s="62">
         <v>28695164.199999999</v>
       </c>
-      <c r="J14" s="47"/>
+      <c r="J14" s="62"/>
       <c r="K14" s="9">
         <f t="shared" si="4"/>
         <v>21707891.717300002</v>
@@ -3970,25 +3969,25 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="112"/>
-      <c r="B15" s="72"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="86"/>
+      <c r="A15" s="122"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="98"/>
       <c r="F15" s="5">
         <f t="shared" si="3"/>
         <v>1.842265107646611</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H15" s="11">
         <v>80</v>
       </c>
-      <c r="I15" s="47">
+      <c r="I15" s="62">
         <v>145778911</v>
       </c>
-      <c r="J15" s="47"/>
+      <c r="J15" s="62"/>
       <c r="K15" s="9">
         <f t="shared" si="4"/>
         <v>109334183.25</v>
@@ -4006,32 +4005,32 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="112"/>
-      <c r="B16" s="72"/>
-      <c r="C16" s="79"/>
-      <c r="D16" s="80"/>
-      <c r="E16" s="87"/>
+      <c r="A16" s="122"/>
+      <c r="B16" s="77"/>
+      <c r="C16" s="84"/>
+      <c r="D16" s="85"/>
+      <c r="E16" s="99"/>
       <c r="F16" s="5">
         <f>H16</f>
         <v>64.989999999999995</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H16" s="11">
         <v>64.989999999999995</v>
       </c>
-      <c r="I16" s="47">
+      <c r="I16" s="62">
         <f>(H16*C12)/100</f>
         <v>7248096.8366</v>
       </c>
-      <c r="J16" s="47"/>
+      <c r="J16" s="62"/>
       <c r="K16" s="9"/>
       <c r="L16" s="12">
         <v>13534750</v>
       </c>
       <c r="M16" s="12">
-        <f t="shared" ref="M13:M16" si="7">+K16-(E36+G36)</f>
+        <f t="shared" ref="M16" si="7">+K16-(E36+G36)</f>
         <v>0</v>
       </c>
       <c r="N16" s="10">
@@ -4040,22 +4039,22 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="50"/>
-      <c r="B17" s="113"/>
-      <c r="C17" s="114">
+      <c r="A17" s="65"/>
+      <c r="B17" s="123"/>
+      <c r="C17" s="124">
         <f>SUM(C12:D12)</f>
         <v>11152634</v>
       </c>
-      <c r="D17" s="115"/>
+      <c r="D17" s="125"/>
       <c r="E17" s="29"/>
       <c r="F17" s="20">
         <f>SUM(F12:F16)</f>
         <v>100</v>
       </c>
-      <c r="G17" s="49"/>
-      <c r="H17" s="50"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="50"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
       <c r="K17" s="21">
         <f>SUM(K12:K12)</f>
         <v>21942042.829999998</v>
@@ -4071,14 +4070,14 @@
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="106" t="s">
+      <c r="A18" s="105" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="107"/>
-      <c r="C18" s="108" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="107"/>
+      <c r="B18" s="106"/>
+      <c r="C18" s="107" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="106"/>
       <c r="E18" s="30"/>
       <c r="F18" s="24" t="s">
         <v>4</v>
@@ -4087,35 +4086,35 @@
         <v>6</v>
       </c>
       <c r="H18" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="I18" s="84" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="73" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" s="95"/>
+      <c r="K18" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="L18" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="92"/>
-      <c r="K18" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="L18" s="27" t="s">
-        <v>24</v>
-      </c>
       <c r="M18" s="27" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="N18" s="26" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="111" t="s">
-        <v>42</v>
-      </c>
-      <c r="B19" s="70"/>
-      <c r="C19" s="75">
+      <c r="A19" s="121" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="75"/>
+      <c r="C19" s="80">
         <v>22126609.300000001</v>
       </c>
-      <c r="D19" s="76"/>
-      <c r="E19" s="85">
+      <c r="D19" s="81"/>
+      <c r="E19" s="97">
         <f>C19-I20</f>
         <v>4425321.8599999994</v>
       </c>
@@ -4124,15 +4123,15 @@
         <v>19.999999999999996</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H19" s="11">
         <v>62.35</v>
       </c>
-      <c r="I19" s="47">
+      <c r="I19" s="62">
         <v>14960000</v>
       </c>
-      <c r="J19" s="47"/>
+      <c r="J19" s="62"/>
       <c r="K19" s="9">
         <f>(I19*C25)/100</f>
         <v>9327560</v>
@@ -4150,26 +4149,26 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="112"/>
-      <c r="B20" s="72"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="87"/>
+      <c r="A20" s="122"/>
+      <c r="B20" s="77"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="99"/>
       <c r="F20" s="5">
         <f>H20</f>
         <v>80</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H20" s="8">
         <v>80</v>
       </c>
-      <c r="I20" s="47">
+      <c r="I20" s="62">
         <f>(H20*C19)/100</f>
         <v>17701287.440000001</v>
       </c>
-      <c r="J20" s="47"/>
+      <c r="J20" s="62"/>
       <c r="K20" s="9"/>
       <c r="L20" s="12">
         <v>18948650</v>
@@ -4184,8 +4183,8 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="50"/>
-      <c r="B21" s="113"/>
+      <c r="A21" s="65"/>
+      <c r="B21" s="123"/>
       <c r="C21" s="104">
         <f>SUM(C19:D19)</f>
         <v>22126609.300000001</v>
@@ -4196,10 +4195,10 @@
         <f>SUM(F19:F20)</f>
         <v>100</v>
       </c>
-      <c r="G21" s="49"/>
-      <c r="H21" s="50"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="50"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="65"/>
       <c r="K21" s="21">
         <f>SUM(K19:K19)</f>
         <v>9327560</v>
@@ -4215,75 +4214,75 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="97" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="98"/>
-      <c r="C23" s="99"/>
+      <c r="A23" s="113" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="114"/>
+      <c r="C23" s="115"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="96" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="96"/>
+      <c r="A24" s="100" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="100"/>
       <c r="C24" s="32">
         <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="124" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="125"/>
+      <c r="A25" s="119" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="120"/>
       <c r="C25" s="32">
         <v>62.35</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="124" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="125"/>
+      <c r="A26" s="119" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" s="120"/>
       <c r="C26" s="32">
         <v>75.650000000000006</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="124" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="125"/>
+      <c r="A27" s="119" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="120"/>
       <c r="C27" s="32">
         <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="95" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="95"/>
-      <c r="C29" s="95"/>
-      <c r="D29" s="95"/>
+      <c r="A29" s="118" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="118"/>
+      <c r="C29" s="118"/>
+      <c r="D29" s="118"/>
       <c r="E29" s="35" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F29" s="35" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G29" s="33" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B30" s="94">
+        <v>34</v>
+      </c>
+      <c r="B30" s="101">
         <f>L5+L12</f>
         <v>5007857500</v>
       </c>
-      <c r="C30" s="94"/>
-      <c r="D30" s="94"/>
+      <c r="C30" s="101"/>
+      <c r="D30" s="101"/>
       <c r="E30" s="12">
         <f>L5</f>
         <v>2436255000</v>
@@ -4299,14 +4298,14 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="94">
+        <v>35</v>
+      </c>
+      <c r="B31" s="101">
         <f>+L6+L13+L19</f>
         <v>833024008.37</v>
       </c>
-      <c r="C31" s="94"/>
-      <c r="D31" s="94"/>
+      <c r="C31" s="101"/>
+      <c r="D31" s="101"/>
       <c r="E31" s="12">
         <f>L6</f>
         <v>7674953.3700000001</v>
@@ -4322,14 +4321,14 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" s="94">
+        <v>36</v>
+      </c>
+      <c r="B32" s="101">
         <f>+L7+L14</f>
         <v>29472555.920000002</v>
       </c>
-      <c r="C32" s="94"/>
-      <c r="D32" s="94"/>
+      <c r="C32" s="101"/>
+      <c r="D32" s="101"/>
       <c r="E32" s="12">
         <f>L7</f>
         <v>13534750</v>
@@ -4345,14 +4344,14 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" s="94">
+        <v>37</v>
+      </c>
+      <c r="B33" s="101">
         <f>+L8+L15</f>
         <v>433112000</v>
       </c>
-      <c r="C33" s="94"/>
-      <c r="D33" s="94"/>
+      <c r="C33" s="101"/>
+      <c r="D33" s="101"/>
       <c r="E33" s="12">
         <f>L8</f>
         <v>243625500</v>
@@ -4368,11 +4367,29 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A5:B10"/>
+    <mergeCell ref="A12:B17"/>
+    <mergeCell ref="A19:B21"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="A2:N2"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="A3:N3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="I13:J13"/>
     <mergeCell ref="I16:J16"/>
     <mergeCell ref="I9:J9"/>
@@ -4380,43 +4397,25 @@
     <mergeCell ref="E5:E9"/>
     <mergeCell ref="C12:D16"/>
     <mergeCell ref="E12:E16"/>
-    <mergeCell ref="C19:D20"/>
-    <mergeCell ref="E19:E20"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="G10:J10"/>
-    <mergeCell ref="A2:N2"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A3:N3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="I4:J4"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="C19:D20"/>
+    <mergeCell ref="E19:E20"/>
     <mergeCell ref="B32:D32"/>
-    <mergeCell ref="A5:B10"/>
-    <mergeCell ref="A12:B17"/>
-    <mergeCell ref="A19:B21"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="G21:J21"/>
     <mergeCell ref="B31:D31"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="G17:J17"/>
     <mergeCell ref="A29:D29"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>